<commit_message>
update Rmd file for Desmarais and generate figures for presentation
also update asfontes data to include new observation
</commit_message>
<xml_diff>
--- a/data/raw/adfontes.xlsx
+++ b/data/raw/adfontes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a836aa78e79a67a3/Documents-TBG/R/workspace/projects/anes-media-bias/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{FC05C402-5433-4D76-8DCF-BCBCC4AD26F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9ACCCCD-F1CA-446E-94A7-646940BD9515}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{FC05C402-5433-4D76-8DCF-BCBCC4AD26F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{695E9B7A-8023-484D-A8CF-AE1FCCE365D3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{87BFB0C0-95A9-48FD-AFEA-2B6506A95FC2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="140">
   <si>
     <t>V201630a</t>
   </si>
@@ -140,12 +140,6 @@
     <t>V201630r</t>
   </si>
   <si>
-    <t>NONE OF THE ABOVE</t>
-  </si>
-  <si>
-    <t>V201630s</t>
-  </si>
-  <si>
     <t>V201631a</t>
   </si>
   <si>
@@ -242,9 +236,6 @@
     <t>SATURDAY NIGHT LIVE (NBC)</t>
   </si>
   <si>
-    <t>V201631s</t>
-  </si>
-  <si>
     <t>V201633a</t>
   </si>
   <si>
@@ -335,9 +326,6 @@
     <t>FRESH AIR (NPR)</t>
   </si>
   <si>
-    <t>V201633r</t>
-  </si>
-  <si>
     <t>V201634a</t>
   </si>
   <si>
@@ -426,18 +414,6 @@
   </si>
   <si>
     <t>NBC NEWS (WWW.NBCNEWS.COM)</t>
-  </si>
-  <si>
-    <t>V201634r</t>
-  </si>
-  <si>
-    <t>OTHER {SPECIFY}</t>
-  </si>
-  <si>
-    <t>V201634s</t>
-  </si>
-  <si>
-    <t>NONE</t>
   </si>
   <si>
     <t>V201636a</t>
@@ -532,6 +508,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -823,7 +803,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -831,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE089E35-6AFB-4977-84C4-DC8F4EB6562A}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,10 +827,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -859,7 +839,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -870,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -887,7 +867,7 @@
         <v>25.67</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -904,7 +884,7 @@
         <v>23.38</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,7 +901,7 @@
         <v>-16.75</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -938,7 +918,7 @@
         <v>-20.309999999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,7 +935,7 @@
         <v>13.22</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -972,7 +952,7 @@
         <v>25.51</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -989,7 +969,7 @@
         <v>12.22</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1006,7 +986,7 @@
         <v>-16.13</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,7 +1003,7 @@
         <v>-13.27</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1040,7 +1020,7 @@
         <v>8.4700000000000006</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,7 +1037,7 @@
         <v>-5.08</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1074,7 +1054,7 @@
         <v>-8.1</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1091,7 +1071,7 @@
         <v>-5.9</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1108,7 +1088,7 @@
         <v>-9.4700000000000006</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,18 +1099,18 @@
         <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,8 +1120,14 @@
       <c r="B19" t="s">
         <v>37</v>
       </c>
+      <c r="C19">
+        <v>36.54</v>
+      </c>
+      <c r="D19">
+        <v>-10.81</v>
+      </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,69 +1138,69 @@
         <v>39</v>
       </c>
       <c r="C20">
-        <v>36.54</v>
+        <v>34.130000000000003</v>
       </c>
       <c r="D20">
-        <v>-10.81</v>
+        <v>-9.2100000000000009</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21">
-        <v>34.130000000000003</v>
-      </c>
-      <c r="D21">
-        <v>-9.2100000000000009</v>
-      </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
+      <c r="C23">
+        <v>48.78</v>
+      </c>
+      <c r="D23">
+        <v>-4.4400000000000004</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
       <c r="C24">
-        <v>48.78</v>
+        <v>42.67</v>
       </c>
       <c r="D24">
-        <v>-4.4400000000000004</v>
+        <v>-8</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,13 +1211,13 @@
         <v>49</v>
       </c>
       <c r="C25">
-        <v>42.67</v>
+        <v>42.11</v>
       </c>
       <c r="D25">
-        <v>-8</v>
+        <v>-4.33</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,13 +1228,13 @@
         <v>51</v>
       </c>
       <c r="C26">
-        <v>42.11</v>
+        <v>41.89</v>
       </c>
       <c r="D26">
-        <v>-4.33</v>
+        <v>-2.78</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,13 +1245,13 @@
         <v>53</v>
       </c>
       <c r="C27">
-        <v>41.89</v>
+        <v>42</v>
       </c>
       <c r="D27">
-        <v>-2.78</v>
+        <v>-1.22</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,13 +1262,13 @@
         <v>55</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>32.56</v>
       </c>
       <c r="D28">
-        <v>-1.22</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,13 +1279,13 @@
         <v>57</v>
       </c>
       <c r="C29">
-        <v>32.56</v>
+        <v>38.4</v>
       </c>
       <c r="D29">
-        <v>21</v>
+        <v>-10</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,13 +1296,13 @@
         <v>59</v>
       </c>
       <c r="C30">
-        <v>38.4</v>
+        <v>22.67</v>
       </c>
       <c r="D30">
-        <v>-10</v>
+        <v>-17.78</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,13 +1313,13 @@
         <v>61</v>
       </c>
       <c r="C31">
-        <v>22.67</v>
+        <v>35.11</v>
       </c>
       <c r="D31">
-        <v>-17.78</v>
+        <v>-13.67</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,13 +1330,13 @@
         <v>63</v>
       </c>
       <c r="C32">
-        <v>35.11</v>
+        <v>46</v>
       </c>
       <c r="D32">
-        <v>-13.67</v>
+        <v>-5.17</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,14 +1346,8 @@
       <c r="B33" t="s">
         <v>65</v>
       </c>
-      <c r="C33">
-        <v>46</v>
-      </c>
-      <c r="D33">
-        <v>-5.17</v>
-      </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1377,8 +1357,14 @@
       <c r="B34" t="s">
         <v>67</v>
       </c>
+      <c r="C34">
+        <v>16.52</v>
+      </c>
+      <c r="D34">
+        <v>26.09</v>
+      </c>
       <c r="E34" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1386,591 +1372,536 @@
         <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="D35">
+        <v>23.44</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36">
-        <v>16.52</v>
+        <v>44.83</v>
       </c>
       <c r="D36">
-        <v>26.09</v>
+        <v>-2.58</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C37">
-        <v>16.649999999999999</v>
+        <v>43.06</v>
       </c>
       <c r="D37">
-        <v>23.44</v>
+        <v>-6.63</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38">
-        <v>44.83</v>
-      </c>
-      <c r="D38">
-        <v>-2.58</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39">
-        <v>43.06</v>
-      </c>
-      <c r="D39">
-        <v>-6.63</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="C40">
+        <v>9.49</v>
+      </c>
+      <c r="D40">
+        <v>31.5</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="C41">
+        <v>14.44</v>
+      </c>
+      <c r="D41">
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42">
-        <v>9.49</v>
-      </c>
-      <c r="D42">
-        <v>31.5</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43">
+        <v>34.56</v>
+      </c>
+      <c r="D43">
         <v>14.44</v>
       </c>
-      <c r="D43">
-        <v>29</v>
-      </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="C44">
+        <v>11.95</v>
+      </c>
+      <c r="D44">
+        <v>28.47</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C45">
+        <v>23</v>
+      </c>
+      <c r="D45">
+        <v>20.87</v>
       </c>
       <c r="E45" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C46">
-        <v>11.95</v>
+        <v>23.61</v>
       </c>
       <c r="D46">
-        <v>28.47</v>
+        <v>-21.11</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47">
-        <v>23</v>
-      </c>
-      <c r="D47">
-        <v>20.87</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48">
-        <v>23.61</v>
+        <v>44.25</v>
       </c>
       <c r="D48">
-        <v>-21.11</v>
+        <v>-5.81</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="C49">
+        <v>42.33</v>
+      </c>
+      <c r="D49">
+        <v>-6.71</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C50">
-        <v>44.25</v>
+        <v>42.42</v>
       </c>
       <c r="D50">
-        <v>-5.81</v>
+        <v>-7.97</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>101</v>
+      </c>
+      <c r="C51">
+        <v>39.65</v>
+      </c>
+      <c r="D51">
+        <v>-11.41</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C52">
-        <v>42.33</v>
+        <v>42.67</v>
       </c>
       <c r="D52">
-        <v>-6.71</v>
+        <v>-7.75</v>
       </c>
       <c r="E52" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C53">
-        <v>42.42</v>
+        <v>30.02</v>
       </c>
       <c r="D53">
-        <v>-7.97</v>
+        <v>15.87</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C54">
-        <v>39.65</v>
+        <v>35.83</v>
       </c>
       <c r="D54">
-        <v>-11.41</v>
+        <v>13.34</v>
       </c>
       <c r="E54" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C55">
-        <v>42.67</v>
+        <v>38.99</v>
       </c>
       <c r="D55">
-        <v>-7.75</v>
+        <v>-8.85</v>
       </c>
       <c r="E55" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C56">
-        <v>30.02</v>
+        <v>42.16</v>
       </c>
       <c r="D56">
-        <v>15.87</v>
+        <v>-8.4600000000000009</v>
       </c>
       <c r="E56" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C57">
-        <v>35.83</v>
+        <v>41.22</v>
       </c>
       <c r="D57">
-        <v>13.34</v>
+        <v>-5.09</v>
       </c>
       <c r="E57" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C58">
-        <v>38.99</v>
+        <v>45.96</v>
       </c>
       <c r="D58">
-        <v>-8.85</v>
+        <v>-2.39</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C59">
-        <v>42.16</v>
+        <v>43.25</v>
       </c>
       <c r="D59">
-        <v>-8.4600000000000009</v>
+        <v>-4.88</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C60">
-        <v>41.22</v>
+        <v>30.67</v>
       </c>
       <c r="D60">
-        <v>-5.09</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="E60" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C61">
-        <v>45.96</v>
+        <v>45.08</v>
       </c>
       <c r="D61">
-        <v>-2.39</v>
+        <v>-3.05</v>
       </c>
       <c r="E61" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C62">
-        <v>43.25</v>
+        <v>43.13</v>
       </c>
       <c r="D62">
-        <v>-4.88</v>
+        <v>-7.75</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C63">
-        <v>30.67</v>
+        <v>45.26</v>
       </c>
       <c r="D63">
-        <v>16.920000000000002</v>
+        <v>-6.68</v>
       </c>
       <c r="E63" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C64">
-        <v>45.08</v>
+        <v>42.67</v>
       </c>
       <c r="D64">
-        <v>-3.05</v>
+        <v>-7.75</v>
       </c>
       <c r="E64" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C65">
-        <v>43.13</v>
+        <v>41.22</v>
       </c>
       <c r="D65">
-        <v>-7.75</v>
+        <v>-5.09</v>
       </c>
       <c r="E65" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C66">
-        <v>45.26</v>
+        <v>44.84</v>
       </c>
       <c r="D66">
-        <v>-6.68</v>
+        <v>5.35</v>
       </c>
       <c r="E66" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="C67">
+        <v>38.99</v>
+      </c>
+      <c r="D67">
+        <v>-8.85</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>132</v>
-      </c>
-      <c r="B68" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69">
-        <v>42.67</v>
-      </c>
-      <c r="D69">
-        <v>-7.75</v>
-      </c>
-      <c r="E69" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
         <v>136</v>
-      </c>
-      <c r="B70" t="s">
-        <v>117</v>
-      </c>
-      <c r="C70">
-        <v>41.22</v>
-      </c>
-      <c r="D70">
-        <v>-5.09</v>
-      </c>
-      <c r="E70" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>137</v>
-      </c>
-      <c r="B71" t="s">
-        <v>138</v>
-      </c>
-      <c r="C71">
-        <v>44.84</v>
-      </c>
-      <c r="D71">
-        <v>5.35</v>
-      </c>
-      <c r="E71" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>139</v>
-      </c>
-      <c r="B72" t="s">
-        <v>140</v>
-      </c>
-      <c r="C72">
-        <v>38.99</v>
-      </c>
-      <c r="D72">
-        <v>-8.85</v>
-      </c>
-      <c r="E72" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>